<commit_message>
updates xls form and README.md
</commit_message>
<xml_diff>
--- a/docs/form.xlsx
+++ b/docs/form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icrucrob/Dropbox/SHARED_FOLDERS/ODK/Example Forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icrucrob/Documents/GitHub/ODK_Fingerprints_Mantra/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A697F-1678-1E4B-87CF-2E56B19DB897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFAA45-D309-5349-8B46-3BD19BACEAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19720" xr2:uid="{B4105C3C-AD41-8E44-BE94-6183AE64A14E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>type</t>
   </si>
@@ -50,13 +50,10 @@
     <t>ex:uk.ac.lshtm.keppel.android.SCAN</t>
   </si>
   <si>
-    <t>Left Thumb</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>L.THUMB</t>
+    <t>finger</t>
   </si>
 </sst>
 </file>
@@ -469,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477F2CDF-7F2A-5742-9608-AECE37A19D7D}">
   <dimension ref="A1:BI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="4"/>
@@ -547,10 +544,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Fixes problem with fingerprint n-char
</commit_message>
<xml_diff>
--- a/docs/form.xlsx
+++ b/docs/form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icrucrob/Documents/GitHub/ODK_Fingerprints_Mantra/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFAA45-D309-5349-8B46-3BD19BACEAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE861C2-F74A-AF4A-8A0B-40C0A81109DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19720" xr2:uid="{B4105C3C-AD41-8E44-BE94-6183AE64A14E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>type</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>finger</t>
+  </si>
+  <si>
+    <t>bind::odk:length</t>
   </si>
 </sst>
 </file>
@@ -466,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477F2CDF-7F2A-5742-9608-AECE37A19D7D}">
   <dimension ref="A1:BI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,6 +497,9 @@
       </c>
       <c r="D1" s="9" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="N1"/>
     </row>
@@ -552,7 +558,9 @@
       <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>10000</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="I3" s="4"/>

</xml_diff>